<commit_message>
commit avant de debug temps 0.0
</commit_message>
<xml_diff>
--- a/tp2/exemple/src/result_glouton1_1.xlsx
+++ b/tp2/exemple/src/result_glouton1_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujiading/Desktop/poly stuff/Algo/TP/swagnalyse/tp2/exemple/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp2\exemple\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4572D4B7-396B-9446-859D-42206B57640F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{697D15FE-DA62-475A-BA7C-80640CCADD28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14500" xr2:uid="{5E1C5933-FED9-854C-841B-467E1B961C4A}"/>
+    <workbookView xWindow="78" yWindow="462" windowWidth="25440" windowHeight="14502" xr2:uid="{5E1C5933-FED9-854C-841B-467E1B961C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -389,16 +389,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D3A866-B3F1-5D4F-A126-3B73E31B27BE}">
   <dimension ref="A1:B270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.34765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,1347 +404,1347 @@
         <v>1.0379999999999799E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.7">
       <c r="B2" s="1">
         <v>7.2800000000000599E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.7">
       <c r="B3" s="1">
         <v>9.1799999999999499E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.7">
       <c r="B4" s="1">
         <v>7.8399999999999997E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.7">
       <c r="B5" s="1">
         <v>7.1400000000000597E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.7">
       <c r="B6" s="1">
         <v>7.3100000000000205E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.7">
       <c r="B7" s="1">
         <v>7.2300000000000099E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.7">
       <c r="B8" s="1">
         <v>8.61E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.7">
       <c r="B9" s="1">
         <v>1.042E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="17.7">
       <c r="B10" s="1">
         <v>8.7899999999999697E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="17.7">
       <c r="B11" s="2">
         <v>7.8000000000001598E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="17.7">
       <c r="B12" s="1">
         <v>1.00000000000002E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="17.7">
       <c r="B13" s="2">
         <v>9.9999999999995898E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="17.7">
       <c r="B14" s="2">
         <v>8.2000000000005598E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="17.7">
       <c r="B15" s="2">
         <v>8.1999999999991802E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="17.7">
       <c r="B16" s="1">
         <v>1.3099999999999901E-4</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="17.7">
       <c r="B17" s="2">
         <v>9.7999999999993898E-5</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="17.7">
       <c r="B18" s="2">
         <v>8.50000000000017E-5</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="17.7">
       <c r="B19" s="2">
         <v>7.7000000000007604E-5</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="17.7">
       <c r="B20" s="2">
         <v>8.50000000000017E-5</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="17.7">
       <c r="B21" s="1">
         <v>3.8400000000000202E-4</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="17.7">
       <c r="B22" s="1">
         <v>3.9300000000000402E-4</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="17.7">
       <c r="B23" s="1">
         <v>3.6299999999998801E-4</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" ht="17.7">
       <c r="B24" s="1">
         <v>5.2100000000000703E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" ht="17.7">
       <c r="B25" s="1">
         <v>3.4400000000000402E-4</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" ht="17.7">
       <c r="B26" s="1">
         <v>3.8300000000000801E-4</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" ht="17.7">
       <c r="B27" s="1">
         <v>4.1300000000000299E-4</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2" ht="17.7">
       <c r="B28" s="1">
         <v>4.2699999999999601E-4</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" ht="17.7">
       <c r="B29" s="1">
         <v>4.9299999999999301E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" ht="17.7">
       <c r="B30" s="1">
         <v>4.5200000000000101E-4</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" ht="17.7">
       <c r="B31" s="2">
         <v>1.80000000000041E-5</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" ht="17.7">
       <c r="B32" s="2">
         <v>2.5999999999998199E-5</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" ht="17.7">
       <c r="B33" s="2">
         <v>1.59999999999951E-5</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" ht="17.7">
       <c r="B34" s="2">
         <v>2.10000000000071E-5</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" ht="17.7">
       <c r="B35" s="2">
         <v>2.4000000000003101E-5</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" ht="17.7">
       <c r="B36" s="2">
         <v>1.89999999999981E-5</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" ht="17.7">
       <c r="B37" s="2">
         <v>1.89999999999981E-5</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" ht="17.7">
       <c r="B38" s="2">
         <v>1.89999999999981E-5</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" ht="17.7">
       <c r="B39" s="2">
         <v>1.89999999999981E-5</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" ht="17.7">
       <c r="B40" s="2">
         <v>1.90000000000051E-5</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" ht="17.7">
       <c r="B41" s="2">
         <v>1.70000000000031E-5</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" ht="17.7">
       <c r="B42" s="2">
         <v>1.69999999999961E-5</v>
       </c>
     </row>
-    <row r="43" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" ht="17.7">
       <c r="B43" s="2">
         <v>2.3000000000002101E-5</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" ht="17.7">
       <c r="B44" s="2">
         <v>1.70000000000031E-5</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" ht="17.7">
       <c r="B45" s="2">
         <v>2.10000000000071E-5</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" ht="17.7">
       <c r="B46" s="2">
         <v>1.90000000000051E-5</v>
       </c>
     </row>
-    <row r="47" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" ht="17.7">
       <c r="B47" s="2">
         <v>1.79999999999971E-5</v>
       </c>
     </row>
-    <row r="48" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" ht="17.7">
       <c r="B48" s="2">
         <v>2.20000000000081E-5</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" ht="17.7">
       <c r="B49" s="2">
         <v>1.90000000000051E-5</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" ht="17.7">
       <c r="B50" s="2">
         <v>1.99999999999991E-5</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" ht="17.7">
       <c r="B51" s="2">
         <v>1.90000000000051E-5</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" ht="17.7">
       <c r="B52" s="2">
         <v>2.10000000000001E-5</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" ht="17.7">
       <c r="B53" s="2">
         <v>1.79999999999971E-5</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" ht="17.7">
       <c r="B54" s="2">
         <v>1.7999999999990199E-5</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" ht="17.7">
       <c r="B55" s="2">
         <v>1.60000000000021E-5</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" ht="17.7">
       <c r="B56" s="2">
         <v>1.69999999999961E-5</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" ht="17.7">
       <c r="B57" s="2">
         <v>1.79999999999971E-5</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" ht="17.7">
       <c r="B58" s="2">
         <v>1.79999999999971E-5</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" ht="17.7">
       <c r="B59" s="2">
         <v>2.00000000000061E-5</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" ht="17.7">
       <c r="B60" s="2">
         <v>1.99999999999991E-5</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" ht="17.7">
       <c r="B61" s="2">
         <v>7.7000000000000598E-5</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" ht="17.7">
       <c r="B62" s="1">
         <v>2.7199999999999398E-4</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" ht="17.7">
       <c r="B63" s="2">
         <v>8.3000000000006598E-5</v>
       </c>
     </row>
-    <row r="64" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" ht="17.7">
       <c r="B64" s="2">
         <v>7.89999999999957E-5</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" ht="17.7">
       <c r="B65" s="2">
         <v>9.1000000000000802E-5</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" ht="17.7">
       <c r="B66" s="2">
         <v>7.2999999999996597E-5</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" ht="17.7">
       <c r="B67" s="2">
         <v>8.1000000000004598E-5</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" ht="17.7">
       <c r="B68" s="2">
         <v>8.0000000000003598E-5</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" ht="17.7">
       <c r="B69" s="2">
         <v>8.19999999999987E-5</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" ht="17.7">
       <c r="B70" s="2">
         <v>7.8000000000001598E-5</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:2" ht="17.7">
       <c r="B71" s="1">
         <v>1.00000000000002E-4</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:2" ht="17.7">
       <c r="B72" s="1">
         <v>1.3699999999999799E-4</v>
       </c>
     </row>
-    <row r="73" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:2" ht="17.7">
       <c r="B73" s="2">
         <v>7.5999999999999598E-5</v>
       </c>
     </row>
-    <row r="74" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2" ht="17.7">
       <c r="B74" s="2">
         <v>9.1000000000000802E-5</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2" ht="17.7">
       <c r="B75" s="1">
         <v>1.8500000000000401E-4</v>
       </c>
     </row>
-    <row r="76" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2" ht="17.7">
       <c r="B76" s="1">
         <v>1.27000000000002E-4</v>
       </c>
     </row>
-    <row r="77" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2" ht="17.7">
       <c r="B77" s="2">
         <v>8.09999999999977E-5</v>
       </c>
     </row>
-    <row r="78" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2" ht="17.7">
       <c r="B78" s="2">
         <v>8.19999999999987E-5</v>
       </c>
     </row>
-    <row r="79" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2" ht="17.7">
       <c r="B79" s="1">
         <v>1.5699999999999701E-4</v>
       </c>
     </row>
-    <row r="80" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:2" ht="17.7">
       <c r="B80" s="1">
         <v>1.11000000000006E-4</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" ht="17.7">
       <c r="B81" s="2">
         <v>8.8999999999998802E-5</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" ht="17.7">
       <c r="B82" s="1">
         <v>1.6000000000000001E-4</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" ht="17.7">
       <c r="B83" s="2">
         <v>8.5999999999995802E-5</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" ht="17.7">
       <c r="B84" s="2">
         <v>8.3000000000013605E-5</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" ht="17.7">
       <c r="B85" s="2">
         <v>8.4999999999994802E-5</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2" ht="17.7">
       <c r="B86" s="2">
         <v>7.79999999999947E-5</v>
       </c>
     </row>
-    <row r="87" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:2" ht="17.7">
       <c r="B87" s="2">
         <v>8.5999999999995802E-5</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:2" ht="17.7">
       <c r="B88" s="2">
         <v>9.4999999999997796E-5</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:2" ht="17.7">
       <c r="B89" s="1">
         <v>1.44999999999992E-4</v>
       </c>
     </row>
-    <row r="90" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:2" ht="17.7">
       <c r="B90" s="1">
         <v>1.1399999999999599E-4</v>
       </c>
     </row>
-    <row r="91" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:2" ht="17.7">
       <c r="B91" s="1">
         <v>7.6199999999999803E-4</v>
       </c>
     </row>
-    <row r="92" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:2" ht="17.7">
       <c r="B92" s="1">
         <v>6.85999999999999E-4</v>
       </c>
     </row>
-    <row r="93" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:2" ht="17.7">
       <c r="B93" s="1">
         <v>8.1599999999999696E-4</v>
       </c>
     </row>
-    <row r="94" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:2" ht="17.7">
       <c r="B94" s="1">
         <v>7.0699999999999897E-4</v>
       </c>
     </row>
-    <row r="95" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:2" ht="17.7">
       <c r="B95" s="1">
         <v>6.8899999999999496E-4</v>
       </c>
     </row>
-    <row r="96" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:2" ht="17.7">
       <c r="B96" s="1">
         <v>1.3829999999999999E-3</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:2" ht="17.7">
       <c r="B97" s="1">
         <v>9.5300000000000202E-4</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:2" ht="17.7">
       <c r="B98" s="1">
         <v>6.8100000000000105E-4</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:2" ht="17.7">
       <c r="B99" s="1">
         <v>1.0330000000000001E-3</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2" ht="17.7">
       <c r="B100" s="1">
         <v>1.32E-3</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:2" ht="17.7">
       <c r="B101" s="1">
         <v>9.6399999999999904E-4</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:2" ht="17.7">
       <c r="B102" s="1">
         <v>7.37000000000001E-4</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:2" ht="17.7">
       <c r="B103" s="1">
         <v>9.6799999999999599E-4</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:2" ht="17.7">
       <c r="B104" s="1">
         <v>1.036E-3</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:2" ht="17.7">
       <c r="B105" s="1">
         <v>7.2400000000000199E-4</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:2" ht="17.7">
       <c r="B106" s="1">
         <v>7.2400000000000199E-4</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:2" ht="17.7">
       <c r="B107" s="1">
         <v>9.9099999999999796E-4</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:2" ht="17.7">
       <c r="B108" s="1">
         <v>9.4799999999998997E-4</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:2" ht="17.7">
       <c r="B109" s="1">
         <v>8.1899999999999996E-4</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:2" ht="17.7">
       <c r="B110" s="1">
         <v>9.7199999999999999E-4</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:2" ht="17.7">
       <c r="B111" s="1">
         <v>9.0700000000000502E-4</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:2" ht="17.7">
       <c r="B112" s="1">
         <v>8.9299999999999796E-4</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:2" ht="17.7">
       <c r="B113" s="1">
         <v>1.0219999999999899E-3</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:2" ht="17.7">
       <c r="B114" s="1">
         <v>7.6400000000000003E-4</v>
       </c>
     </row>
-    <row r="115" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:2" ht="17.7">
       <c r="B115" s="1">
         <v>7.1600000000000103E-4</v>
       </c>
     </row>
-    <row r="116" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:2" ht="17.7">
       <c r="B116" s="1">
         <v>7.3200000000000305E-4</v>
       </c>
     </row>
-    <row r="117" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:2" ht="17.7">
       <c r="B117" s="1">
         <v>7.8299999999999897E-4</v>
       </c>
     </row>
-    <row r="118" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:2" ht="17.7">
       <c r="B118" s="1">
         <v>8.8900000000000003E-4</v>
       </c>
     </row>
-    <row r="119" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:2" ht="17.7">
       <c r="B119" s="1">
         <v>9.4299999999999202E-4</v>
       </c>
     </row>
-    <row r="120" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:2" ht="17.7">
       <c r="B120" s="1">
         <v>1.06999999999999E-3</v>
       </c>
     </row>
-    <row r="121" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:2" ht="17.7">
       <c r="B121" s="2">
         <v>3.30000000000052E-5</v>
       </c>
     </row>
-    <row r="122" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:2" ht="17.7">
       <c r="B122" s="2">
         <v>2.5999999999998199E-5</v>
       </c>
     </row>
-    <row r="123" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:2" ht="17.7">
       <c r="B123" s="2">
         <v>3.1999999999997302E-5</v>
       </c>
     </row>
-    <row r="124" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:2" ht="17.7">
       <c r="B124" s="2">
         <v>2.2000000000001101E-5</v>
       </c>
     </row>
-    <row r="125" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:2" ht="17.7">
       <c r="B125" s="2">
         <v>2.3999999999996199E-5</v>
       </c>
     </row>
-    <row r="126" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:2" ht="17.7">
       <c r="B126" s="2">
         <v>2.5999999999998199E-5</v>
       </c>
     </row>
-    <row r="127" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:2" ht="17.7">
       <c r="B127" s="2">
         <v>2.3000000000002101E-5</v>
       </c>
     </row>
-    <row r="128" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:2" ht="17.7">
       <c r="B128" s="2">
         <v>3.00000000000022E-5</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:2" ht="17.7">
       <c r="B129" s="2">
         <v>2.5000000000004101E-5</v>
       </c>
     </row>
-    <row r="130" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:2" ht="17.7">
       <c r="B130" s="2">
         <v>2.3000000000002101E-5</v>
       </c>
     </row>
-    <row r="131" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:2" ht="17.7">
       <c r="B131" s="2">
         <v>2.4999999999997199E-5</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:2" ht="17.7">
       <c r="B132" s="2">
         <v>2.4999999999997199E-5</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:2" ht="17.7">
       <c r="B133" s="2">
         <v>4.3000000000001303E-5</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:2" ht="17.7">
       <c r="B134" s="2">
         <v>2.8999999999994301E-5</v>
       </c>
     </row>
-    <row r="135" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:2" ht="17.7">
       <c r="B135" s="2">
         <v>2.6999999999999199E-5</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:2" ht="17.7">
       <c r="B136" s="2">
         <v>3.7000000000002302E-5</v>
       </c>
     </row>
-    <row r="137" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:2" ht="17.7">
       <c r="B137" s="2">
         <v>2.3999999999996199E-5</v>
       </c>
     </row>
-    <row r="138" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:2" ht="17.7">
       <c r="B138" s="2">
         <v>3.7000000000002302E-5</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:2" ht="17.7">
       <c r="B139" s="2">
         <v>2.8000000000007101E-5</v>
       </c>
     </row>
-    <row r="140" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:2" ht="17.7">
       <c r="B140" s="2">
         <v>2.5999999999998199E-5</v>
       </c>
     </row>
-    <row r="141" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:2" ht="17.7">
       <c r="B141" s="2">
         <v>2.3999999999996199E-5</v>
       </c>
     </row>
-    <row r="142" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:2" ht="17.7">
       <c r="B142" s="2">
         <v>3.4999999999993302E-5</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:2" ht="17.7">
       <c r="B143" s="2">
         <v>2.5999999999998199E-5</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:2" ht="17.7">
       <c r="B144" s="2">
         <v>3.4999999999993302E-5</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:2" ht="17.7">
       <c r="B145" s="2">
         <v>2.5000000000004101E-5</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:2" ht="17.7">
       <c r="B146" s="2">
         <v>2.5000000000004101E-5</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:2" ht="17.7">
       <c r="B147" s="2">
         <v>2.5999999999991301E-5</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:2" ht="17.7">
       <c r="B148" s="2">
         <v>2.4000000000003101E-5</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:2" ht="17.7">
       <c r="B149" s="2">
         <v>2.6999999999992301E-5</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:2" ht="17.7">
       <c r="B150" s="2">
         <v>2.5999999999998199E-5</v>
       </c>
     </row>
-    <row r="151" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:2" ht="17.7">
       <c r="B151" s="1">
         <v>1.42999999999997E-4</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:2" ht="17.7">
       <c r="B152" s="1">
         <v>1.37999999999992E-4</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:2" ht="17.7">
       <c r="B153" s="1">
         <v>1.33000000000008E-4</v>
       </c>
     </row>
-    <row r="154" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:2" ht="17.7">
       <c r="B154" s="1">
         <v>1.4500000000000599E-4</v>
       </c>
     </row>
-    <row r="155" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:2" ht="17.7">
       <c r="B155" s="1">
         <v>2.6600000000000202E-4</v>
       </c>
     </row>
-    <row r="156" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:2" ht="17.7">
       <c r="B156" s="1">
         <v>1.3499999999999599E-4</v>
       </c>
     </row>
-    <row r="157" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:2" ht="17.7">
       <c r="B157" s="1">
         <v>1.4100000000000199E-4</v>
       </c>
     </row>
-    <row r="158" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:2" ht="17.7">
       <c r="B158" s="1">
         <v>2.0399999999999501E-4</v>
       </c>
     </row>
-    <row r="159" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:2" ht="17.7">
       <c r="B159" s="1">
         <v>1.6399999999999E-4</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:2" ht="17.7">
       <c r="B160" s="1">
         <v>1.5699999999999701E-4</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:2" ht="17.7">
       <c r="B161" s="1">
         <v>2.4999999999999301E-4</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:2" ht="17.7">
       <c r="B162" s="1">
         <v>1.5700000000000401E-4</v>
       </c>
     </row>
-    <row r="163" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:2" ht="17.7">
       <c r="B163" s="1">
         <v>1.5500000000000201E-4</v>
       </c>
     </row>
-    <row r="164" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:2" ht="17.7">
       <c r="B164" s="1">
         <v>1.5799999999999801E-4</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:2" ht="17.7">
       <c r="B165" s="1">
         <v>1.5699999999999701E-4</v>
       </c>
     </row>
-    <row r="166" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:2" ht="17.7">
       <c r="B166" s="1">
         <v>1.7599999999999501E-4</v>
       </c>
     </row>
-    <row r="167" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:2" ht="17.7">
       <c r="B167" s="1">
         <v>3.1400000000000102E-4</v>
       </c>
     </row>
-    <row r="168" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:2" ht="17.7">
       <c r="B168" s="1">
         <v>2.88999999999997E-4</v>
       </c>
     </row>
-    <row r="169" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:2" ht="17.7">
       <c r="B169" s="1">
         <v>3.0199999999999601E-4</v>
       </c>
     </row>
-    <row r="170" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:2" ht="17.7">
       <c r="B170" s="1">
         <v>1.6399999999999699E-4</v>
       </c>
     </row>
-    <row r="171" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:2" ht="17.7">
       <c r="B171" s="1">
         <v>1.5099999999999801E-4</v>
       </c>
     </row>
-    <row r="172" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:2" ht="17.7">
       <c r="B172" s="1">
         <v>1.51000000000005E-4</v>
       </c>
     </row>
-    <row r="173" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:2" ht="17.7">
       <c r="B173" s="1">
         <v>1.6500000000000501E-4</v>
       </c>
     </row>
-    <row r="174" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:2" ht="17.7">
       <c r="B174" s="1">
         <v>1.5599999999999601E-4</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:2" ht="17.7">
       <c r="B175" s="1">
         <v>1.46E-4</v>
       </c>
     </row>
-    <row r="176" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:2" ht="17.7">
       <c r="B176" s="1">
         <v>1.50000000000004E-4</v>
       </c>
     </row>
-    <row r="177" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:2" ht="17.7">
       <c r="B177" s="1">
         <v>1.6699999999999999E-4</v>
       </c>
     </row>
-    <row r="178" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:2" ht="17.7">
       <c r="B178" s="1">
         <v>1.49000000000003E-4</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:2" ht="17.7">
       <c r="B179" s="1">
         <v>1.7999999999999199E-4</v>
       </c>
     </row>
-    <row r="180" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:2" ht="17.7">
       <c r="B180" s="1">
         <v>1.4500000000000599E-4</v>
       </c>
     </row>
-    <row r="181" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:2" ht="17.7">
       <c r="B181" s="1">
         <v>1.42099999999999E-3</v>
       </c>
     </row>
-    <row r="182" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:2" ht="17.7">
       <c r="B182" s="1">
         <v>1.5869999999999899E-3</v>
       </c>
     </row>
-    <row r="183" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:2" ht="17.7">
       <c r="B183" s="1">
         <v>1.397E-3</v>
       </c>
     </row>
-    <row r="184" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:2" ht="17.7">
       <c r="B184" s="1">
         <v>1.4480000000000001E-3</v>
       </c>
     </row>
-    <row r="185" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:2" ht="17.7">
       <c r="B185" s="1">
         <v>1.503E-3</v>
       </c>
     </row>
-    <row r="186" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:2" ht="17.7">
       <c r="B186" s="1">
         <v>1.4469999999999999E-3</v>
       </c>
     </row>
-    <row r="187" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:2" ht="17.7">
       <c r="B187" s="1">
         <v>1.4119999999999901E-3</v>
       </c>
     </row>
-    <row r="188" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:2" ht="17.7">
       <c r="B188" s="1">
         <v>1.9579999999999901E-3</v>
       </c>
     </row>
-    <row r="189" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:2" ht="17.7">
       <c r="B189" s="1">
         <v>1.5299999999999999E-3</v>
       </c>
     </row>
-    <row r="190" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:2" ht="17.7">
       <c r="B190" s="1">
         <v>1.8009999999999899E-3</v>
       </c>
     </row>
-    <row r="191" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:2" ht="17.7">
       <c r="B191" s="1">
         <v>1.359E-3</v>
       </c>
     </row>
-    <row r="192" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:2" ht="17.7">
       <c r="B192" s="1">
         <v>1.454E-3</v>
       </c>
     </row>
-    <row r="193" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:2" ht="17.7">
       <c r="B193" s="1">
         <v>1.3519999999999899E-3</v>
       </c>
     </row>
-    <row r="194" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:2" ht="17.7">
       <c r="B194" s="1">
         <v>1.3879999999999999E-3</v>
       </c>
     </row>
-    <row r="195" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:2" ht="17.7">
       <c r="B195" s="1">
         <v>1.4859999999999899E-3</v>
       </c>
     </row>
-    <row r="196" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:2" ht="17.7">
       <c r="B196" s="1">
         <v>1.3889999999999901E-3</v>
       </c>
     </row>
-    <row r="197" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:2" ht="17.7">
       <c r="B197" s="1">
         <v>1.8680000000000001E-3</v>
       </c>
     </row>
-    <row r="198" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:2" ht="17.7">
       <c r="B198" s="1">
         <v>2.1689999999999999E-3</v>
       </c>
     </row>
-    <row r="199" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:2" ht="17.7">
       <c r="B199" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="200" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:2" ht="17.7">
       <c r="B200" s="1">
         <v>1.7309999999999999E-3</v>
       </c>
     </row>
-    <row r="201" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:2" ht="17.7">
       <c r="B201" s="1">
         <v>1.681E-3</v>
       </c>
     </row>
-    <row r="202" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:2" ht="17.7">
       <c r="B202" s="1">
         <v>2.5600000000000002E-3</v>
       </c>
     </row>
-    <row r="203" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:2" ht="17.7">
       <c r="B203" s="1">
         <v>1.49599999999999E-3</v>
       </c>
     </row>
-    <row r="204" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:2" ht="17.7">
       <c r="B204" s="1">
         <v>1.43099999999999E-3</v>
       </c>
     </row>
-    <row r="205" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:2" ht="17.7">
       <c r="B205" s="1">
         <v>1.926E-3</v>
       </c>
     </row>
-    <row r="206" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:2" ht="17.7">
       <c r="B206" s="1">
         <v>1.40999999999999E-3</v>
       </c>
     </row>
-    <row r="207" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:2" ht="17.7">
       <c r="B207" s="1">
         <v>1.4679999999999999E-3</v>
       </c>
     </row>
-    <row r="208" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:2" ht="17.7">
       <c r="B208" s="1">
         <v>1.3569999999999999E-3</v>
       </c>
     </row>
-    <row r="209" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:2" ht="17.7">
       <c r="B209" s="1">
         <v>1.7619999999999899E-3</v>
       </c>
     </row>
-    <row r="210" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:2" ht="17.7">
       <c r="B210" s="1">
         <v>1.79499999999999E-3</v>
       </c>
     </row>
-    <row r="211" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:2" ht="17.7">
       <c r="B211" s="2">
         <v>4.5999999999997398E-5</v>
       </c>
     </row>
-    <row r="212" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:2" ht="17.7">
       <c r="B212" s="2">
         <v>4.2999999999994398E-5</v>
       </c>
     </row>
-    <row r="213" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:2" ht="17.7">
       <c r="B213" s="2">
         <v>5.6999999999994501E-5</v>
       </c>
     </row>
-    <row r="214" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:2" ht="17.7">
       <c r="B214" s="2">
         <v>6.0999999999991603E-5</v>
       </c>
     </row>
-    <row r="215" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:2" ht="17.7">
       <c r="B215" s="2">
         <v>4.2999999999994398E-5</v>
       </c>
     </row>
-    <row r="216" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:2" ht="17.7">
       <c r="B216" s="2">
         <v>4.4999999999996398E-5</v>
       </c>
     </row>
-    <row r="217" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:2" ht="17.7">
       <c r="B217" s="2">
         <v>4.4999999999996398E-5</v>
       </c>
     </row>
-    <row r="218" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:2" ht="17.7">
       <c r="B218" s="2">
         <v>4.5999999999990398E-5</v>
       </c>
     </row>
-    <row r="219" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:2" ht="17.7">
       <c r="B219" s="1">
         <v>1.4200000000000299E-4</v>
       </c>
     </row>
-    <row r="220" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:2" ht="17.7">
       <c r="B220" s="2">
         <v>6.1999999999999501E-5</v>
       </c>
     </row>
-    <row r="221" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:2" ht="17.7">
       <c r="B221" s="2">
         <v>4.4999999999996398E-5</v>
       </c>
     </row>
-    <row r="222" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:2" ht="17.7">
       <c r="B222" s="2">
         <v>4.5999999999990398E-5</v>
       </c>
     </row>
-    <row r="223" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:2" ht="17.7">
       <c r="B223" s="2">
         <v>4.5999999999997398E-5</v>
       </c>
     </row>
-    <row r="224" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:2" ht="17.7">
       <c r="B224" s="2">
         <v>4.7000000000005303E-5</v>
       </c>
     </row>
-    <row r="225" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:2" ht="17.7">
       <c r="B225" s="2">
         <v>5.0000000000001398E-5</v>
       </c>
     </row>
-    <row r="226" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:2" ht="17.7">
       <c r="B226" s="2">
         <v>4.9999999999994398E-5</v>
       </c>
     </row>
-    <row r="227" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:2" ht="17.7">
       <c r="B227" s="2">
         <v>4.9000000000000398E-5</v>
       </c>
     </row>
-    <row r="228" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:2" ht="17.7">
       <c r="B228" s="2">
         <v>4.9000000000000398E-5</v>
       </c>
     </row>
-    <row r="229" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:2" ht="17.7">
       <c r="B229" s="2">
         <v>4.7999999999992398E-5</v>
       </c>
     </row>
-    <row r="230" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:2" ht="17.7">
       <c r="B230" s="2">
         <v>5.6999999999994501E-5</v>
       </c>
     </row>
-    <row r="231" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:2" ht="17.7">
       <c r="B231" s="2">
         <v>4.6999999999998398E-5</v>
       </c>
     </row>
-    <row r="232" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:2" ht="17.7">
       <c r="B232" s="2">
         <v>4.5999999999997398E-5</v>
       </c>
     </row>
-    <row r="233" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:2" ht="17.7">
       <c r="B233" s="2">
         <v>4.4000000000002303E-5</v>
       </c>
     </row>
-    <row r="234" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:2" ht="17.7">
       <c r="B234" s="2">
         <v>5.8000000000002399E-5</v>
       </c>
     </row>
-    <row r="235" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:2" ht="17.7">
       <c r="B235" s="2">
         <v>5.0000000000008303E-5</v>
       </c>
     </row>
-    <row r="236" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:2" ht="17.7">
       <c r="B236" s="2">
         <v>5.1000000000002398E-5</v>
       </c>
     </row>
-    <row r="237" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:2" ht="17.7">
       <c r="B237" s="2">
         <v>4.5999999999990398E-5</v>
       </c>
     </row>
-    <row r="238" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:2" ht="17.7">
       <c r="B238" s="2">
         <v>4.7999999999992398E-5</v>
       </c>
     </row>
-    <row r="239" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:2" ht="17.7">
       <c r="B239" s="2">
         <v>4.6999999999998398E-5</v>
       </c>
     </row>
-    <row r="240" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:2" ht="17.7">
       <c r="B240" s="2">
         <v>4.5999999999997398E-5</v>
       </c>
     </row>
-    <row r="241" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:2" ht="17.7">
       <c r="B241" s="1">
         <v>3.5000000000000298E-4</v>
       </c>
     </row>
-    <row r="242" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:2" ht="17.7">
       <c r="B242" s="1">
         <v>3.4599999999999898E-4</v>
       </c>
     </row>
-    <row r="243" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:2" ht="17.7">
       <c r="B243" s="1">
         <v>3.5799999999999699E-4</v>
       </c>
     </row>
-    <row r="244" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:2" ht="17.7">
       <c r="B244" s="1">
         <v>3.65999999999998E-4</v>
       </c>
     </row>
-    <row r="245" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:2" ht="17.7">
       <c r="B245" s="1">
         <v>3.6099999999999999E-4</v>
       </c>
     </row>
-    <row r="246" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:2" ht="17.7">
       <c r="B246" s="1">
         <v>3.3299999999999899E-4</v>
       </c>
     </row>
-    <row r="247" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:2" ht="17.7">
       <c r="B247" s="1">
         <v>3.6599999999999101E-4</v>
       </c>
     </row>
-    <row r="248" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:2" ht="17.7">
       <c r="B248" s="1">
         <v>3.5200000000000498E-4</v>
       </c>
     </row>
-    <row r="249" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:2" ht="17.7">
       <c r="B249" s="1">
         <v>4.3700000000000601E-4</v>
       </c>
     </row>
-    <row r="250" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:2" ht="17.7">
       <c r="B250" s="1">
         <v>3.9400000000000502E-4</v>
       </c>
     </row>
-    <row r="251" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:2" ht="17.7">
       <c r="B251" s="1">
         <v>3.8399999999998798E-4</v>
       </c>
     </row>
-    <row r="252" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:2" ht="17.7">
       <c r="B252" s="1">
         <v>4.6300000000000502E-4</v>
       </c>
     </row>
-    <row r="253" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:2" ht="17.7">
       <c r="B253" s="1">
         <v>3.4699999999999998E-4</v>
       </c>
     </row>
-    <row r="254" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:2" ht="17.7">
       <c r="B254" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="255" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:2" ht="17.7">
       <c r="B255" s="1">
         <v>3.5600000000000199E-4</v>
       </c>
     </row>
-    <row r="256" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:2" ht="17.7">
       <c r="B256" s="1">
         <v>3.6699999999999201E-4</v>
       </c>
     </row>
-    <row r="257" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:2" ht="17.7">
       <c r="B257" s="1">
         <v>3.66999999999999E-4</v>
       </c>
     </row>
-    <row r="258" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:2" ht="17.7">
       <c r="B258" s="1">
         <v>3.8100000000000601E-4</v>
       </c>
     </row>
-    <row r="259" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:2" ht="17.7">
       <c r="B259" s="1">
         <v>3.68E-4</v>
       </c>
     </row>
-    <row r="260" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:2" ht="17.7">
       <c r="B260" s="1">
         <v>3.7899999999999702E-4</v>
       </c>
     </row>
-    <row r="261" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:2" ht="17.7">
       <c r="B261" s="1">
         <v>4.0700000000000398E-4</v>
       </c>
     </row>
-    <row r="262" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:2" ht="17.7">
       <c r="B262" s="1">
         <v>3.4499999999999798E-4</v>
       </c>
     </row>
-    <row r="263" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:2" ht="17.7">
       <c r="B263" s="1">
         <v>3.5200000000000498E-4</v>
       </c>
     </row>
-    <row r="264" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:2" ht="17.7">
       <c r="B264" s="1">
         <v>4.4999999999999901E-4</v>
       </c>
     </row>
-    <row r="265" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:2" ht="17.7">
       <c r="B265" s="1">
         <v>3.73000000000005E-4</v>
       </c>
     </row>
-    <row r="266" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:2" ht="17.7">
       <c r="B266" s="1">
         <v>3.8300000000000102E-4</v>
       </c>
     </row>
-    <row r="267" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:2" ht="17.7">
       <c r="B267" s="1">
         <v>3.3000000000000298E-4</v>
       </c>
     </row>
-    <row r="268" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:2" ht="17.7">
       <c r="B268" s="1">
         <v>3.3700000000000299E-4</v>
       </c>
     </row>
-    <row r="269" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:2" ht="17.7">
       <c r="B269" s="1">
         <v>3.6800000000000699E-4</v>
       </c>
     </row>
-    <row r="270" spans="2:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:2" ht="17.7">
       <c r="B270" s="1">
         <v>3.7500000000000001E-4</v>
       </c>

</xml_diff>